<commit_message>
add device id validation
</commit_message>
<xml_diff>
--- a/public/employee_import.xlsx
+++ b/public/employee_import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qoin\Documents\rendi\Kuliah UEU\Semester 3\Tugas Akhir 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\rendi\attendance_mgi\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FFAE57-C59E-4C8A-BA11-5D69C7F9744C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CCA7B5-7BF7-4938-A22C-06DFA86F7FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>0098001</t>
   </si>
@@ -82,6 +82,24 @@
   </si>
   <si>
     <t>Marketing</t>
+  </si>
+  <si>
+    <t>device_id</t>
+  </si>
+  <si>
+    <t>dsf1344324</t>
+  </si>
+  <si>
+    <t>dsf434242</t>
+  </si>
+  <si>
+    <t>assacds343</t>
+  </si>
+  <si>
+    <t>cbfd14324</t>
+  </si>
+  <si>
+    <t>vdbdf343</t>
   </si>
 </sst>
 </file>
@@ -502,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,9 +532,10 @@
     <col min="3" max="3" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="23.77734375" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -535,8 +554,11 @@
       <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -555,8 +577,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -575,8 +600,11 @@
       <c r="F3" s="1">
         <v>2</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -595,8 +623,11 @@
       <c r="F4" s="1">
         <v>3</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -615,8 +646,11 @@
       <c r="F5" s="1">
         <v>4</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -634,6 +668,9 @@
       </c>
       <c r="F6" s="1">
         <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>